<commit_message>
Exception Tweaking and Validation
</commit_message>
<xml_diff>
--- a/src/main/resources/SampleHRL.xlsx
+++ b/src/main/resources/SampleHRL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\IntellijProjects\exceleratormaven\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E45A5F11-93FC-47EF-B885-94DD821C32E6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89AB4B45-70BB-4ACB-8A1A-FF7CCA09AB0A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17268" windowHeight="5910" xr2:uid="{4C868800-59AB-4C70-858F-FE6BD2C3714C}"/>
   </bookViews>
@@ -27,58 +27,58 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
   <si>
+    <t>Component_HRL</t>
+  </si>
+  <si>
+    <t>Position</t>
+  </si>
+  <si>
+    <t>asofdate</t>
+  </si>
+  <si>
+    <t>Top</t>
+  </si>
+  <si>
+    <t>Bottom</t>
+  </si>
+  <si>
+    <t>HRL1</t>
+  </si>
+  <si>
+    <t>HRL2</t>
+  </si>
+  <si>
+    <t>Component1</t>
+  </si>
+  <si>
+    <t>Component2</t>
+  </si>
+  <si>
+    <t>Name1</t>
+  </si>
+  <si>
+    <t>Name2</t>
+  </si>
+  <si>
+    <t>21/07/1989</t>
+  </si>
+  <si>
+    <t>21/07/1999</t>
+  </si>
+  <si>
+    <t>Name3</t>
+  </si>
+  <si>
+    <t>Component3</t>
+  </si>
+  <si>
+    <t>HRL3</t>
+  </si>
+  <si>
+    <t>Sub_Componentt2</t>
+  </si>
+  <si>
     <t>name</t>
-  </si>
-  <si>
-    <t>Sub_Component</t>
-  </si>
-  <si>
-    <t>Component_HRL</t>
-  </si>
-  <si>
-    <t>Position</t>
-  </si>
-  <si>
-    <t>asofdate</t>
-  </si>
-  <si>
-    <t>Top</t>
-  </si>
-  <si>
-    <t>Bottom</t>
-  </si>
-  <si>
-    <t>HRL1</t>
-  </si>
-  <si>
-    <t>HRL2</t>
-  </si>
-  <si>
-    <t>Component1</t>
-  </si>
-  <si>
-    <t>Component2</t>
-  </si>
-  <si>
-    <t>Name1</t>
-  </si>
-  <si>
-    <t>Name2</t>
-  </si>
-  <si>
-    <t>21/07/1989</t>
-  </si>
-  <si>
-    <t>21/07/1999</t>
-  </si>
-  <si>
-    <t>Name3</t>
-  </si>
-  <si>
-    <t>Component3</t>
-  </si>
-  <si>
-    <t>HRL3</t>
   </si>
 </sst>
 </file>
@@ -451,9 +451,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{230B47E4-8C75-4CAC-A6AC-EA93218A5A64}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
@@ -464,67 +462,67 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="B2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="B3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
         <v>15</v>
       </c>
-      <c r="B4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" t="s">
-        <v>17</v>
-      </c>
       <c r="E4" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -534,6 +532,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="94f3f65c-3f9f-412a-a356-4ab058884b3b" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010056D4A1DDDE980741AE1E1A2E53C6A608" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c599adc88a24426b45c0773bae5204cb">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="94f3f65c-3f9f-412a-a356-4ab058884b3b" xmlns:ns4="12c7b69a-64b5-4ae9-80be-9b7818b0bfc8" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a0c5e4b90eef130f24a6dd0aa1559181" ns3:_="" ns4:_="">
     <xsd:import namespace="94f3f65c-3f9f-412a-a356-4ab058884b3b"/>
@@ -768,24 +783,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="94f3f65c-3f9f-412a-a356-4ab058884b3b" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{98B54545-7ABF-4847-8DB6-11602091C6E4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="12c7b69a-64b5-4ae9-80be-9b7818b0bfc8"/>
+    <ds:schemaRef ds:uri="94f3f65c-3f9f-412a-a356-4ab058884b3b"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2C4DB926-1151-45B6-9C14-6E2D302E6405}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{19ACFDF1-5A1C-4EAC-8D71-29A359212992}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -802,29 +825,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2C4DB926-1151-45B6-9C14-6E2D302E6405}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{98B54545-7ABF-4847-8DB6-11602091C6E4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="12c7b69a-64b5-4ae9-80be-9b7818b0bfc8"/>
-    <ds:schemaRef ds:uri="94f3f65c-3f9f-412a-a356-4ab058884b3b"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>